<commit_message>
spreadsheet and tooltiptext improvement
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Category 01.xlsx
+++ b/src/main/resources/spreadsheetFiles/Category 01.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fieldnames" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="category" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="URL" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="color" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="test" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,50 +24,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">Internet #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet #4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wikipedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expasy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duckduckgo</t>
+  </si>
   <si>
     <t xml:space="preserve">Drives</t>
   </si>
   <si>
-    <t xml:space="preserve">Internet #1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internet #2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intranet</t>
   </si>
   <si>
-    <t xml:space="preserve">C:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expasy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Router</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biocentury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gapminder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google Datasearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaggle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OurWorldInData</t>
-  </si>
-  <si>
     <t xml:space="preserve">app1</t>
   </si>
   <si>
@@ -79,7 +68,7 @@
     <t xml:space="preserve">intra1</t>
   </si>
   <si>
-    <t xml:space="preserve">C:\</t>
+    <t xml:space="preserve">www.google.de</t>
   </si>
   <si>
     <t xml:space="preserve">www.github.com</t>
@@ -91,24 +80,6 @@
     <t xml:space="preserve">https://192.168.178.1/</t>
   </si>
   <si>
-    <t xml:space="preserve">D:\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.bio-century.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gapminder.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://datasetsearch.research.google.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.kaggle.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ourworldindata.org/</t>
-  </si>
-  <si>
     <t xml:space="preserve">246,194,62</t>
   </si>
   <si>
@@ -118,7 +89,7 @@
     <t xml:space="preserve">250,250,250</t>
   </si>
   <si>
-    <t xml:space="preserve">231,74,59</t>
+    <t xml:space="preserve">asdfsafd</t>
   </si>
 </sst>
 </file>
@@ -129,11 +100,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,12 +126,6 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -237,15 +203,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,7 +312,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -355,7 +321,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -383,47 +349,31 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Expasy"/>
-    <hyperlink ref="C3" r:id="rId2" display="Gapminder"/>
-    <hyperlink ref="C4" r:id="rId3" display="Google Datasearch"/>
-    <hyperlink ref="C5" r:id="rId4" display="Kaggle"/>
-    <hyperlink ref="C6" r:id="rId5" display="OurWorldInData"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -443,73 +393,61 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
   </sheetData>
@@ -531,7 +469,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,73 +482,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="www.github.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://192.168.178.1/"/>
-    <hyperlink ref="B3" r:id="rId3" display="www.bio-century.net"/>
+    <hyperlink ref="A2" r:id="rId1" display="www.google.de"/>
+    <hyperlink ref="B2" r:id="rId2" display="www.github.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://192.168.178.1/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -629,73 +555,61 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="8"/>
     </row>
   </sheetData>
@@ -707,4 +621,33 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working, but needs to be bugfixed
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Category 01.xlsx
+++ b/src/main/resources/spreadsheetFiles/Category 01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="fieldnames" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t xml:space="preserve">Internet #1</t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">Internet #3</t>
   </si>
   <si>
-    <t xml:space="preserve">Internet #4</t>
-  </si>
-  <si>
     <t xml:space="preserve">wikipedia</t>
   </si>
   <si>
@@ -50,36 +47,30 @@
     <t xml:space="preserve">duckduckgo</t>
   </si>
   <si>
-    <t xml:space="preserve">Drives</t>
+    <t xml:space="preserve">inet1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inet2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inet3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.google.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.github.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.expasy.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://duckduckgo.com/</t>
   </si>
   <si>
     <t xml:space="preserve">Intranet</t>
   </si>
   <si>
-    <t xml:space="preserve">app1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inet1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inet2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intra1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.google.de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.github.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.expasy.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://192.168.178.1/</t>
-  </si>
-  <si>
     <t xml:space="preserve">246,194,62</t>
   </si>
   <si>
@@ -89,7 +80,7 @@
     <t xml:space="preserve">250,250,250</t>
   </si>
   <si>
-    <t xml:space="preserve">asdfsafd</t>
+    <t xml:space="preserve">comment1</t>
   </si>
 </sst>
 </file>
@@ -100,7 +91,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -133,6 +124,21 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -194,7 +200,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,15 +221,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,8 +329,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,7 +339,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -331,25 +349,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
@@ -372,9 +392,6 @@
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Expasy"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -393,41 +410,43 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -469,148 +488,70 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="www.google.de"/>
-    <hyperlink ref="B2" r:id="rId2" display="www.github.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://192.168.178.1/"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -623,22 +564,110 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="D1:D2 H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automatic read-in of number of columns and rows and autoformatting of tabbedpanels
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheetFiles/Category 01.xlsx
+++ b/src/main/resources/spreadsheetFiles/Category 01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t xml:space="preserve">Internet #1</t>
   </si>
@@ -330,7 +330,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,17 +362,15 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -410,7 +408,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -488,7 +486,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,7 +570,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,7 +647,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="D1:D2 H12"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>